<commit_message>
sua diem lan 2
</commit_message>
<xml_diff>
--- a/Diem/Nhom 3.xlsx
+++ b/Diem/Nhom 3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -360,10 +360,10 @@
     <t>Lê Hồng Ngọc</t>
   </si>
   <si>
-    <t xml:space="preserve">0812050 </t>
-  </si>
-  <si>
     <t xml:space="preserve">0812341 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0812190  </t>
   </si>
 </sst>
 </file>
@@ -730,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35:C39"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39:C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1135,7 +1135,7 @@
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>112</v>
@@ -1183,7 +1183,7 @@
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>113</v>
@@ -1873,7 +1873,7 @@
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>112</v>
@@ -1921,7 +1921,7 @@
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>113</v>
@@ -2207,8 +2207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35:C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2612,7 +2612,7 @@
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>112</v>
@@ -2660,7 +2660,7 @@
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>113</v>

</xml_diff>

<commit_message>
Đổi tên các sheet cho dễ theo dõi
</commit_message>
<xml_diff>
--- a/Diem/Nhom 3.xlsx
+++ b/Diem/Nhom 3.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Version Control" sheetId="1" r:id="rId1"/>
+    <sheet name="Project Plan" sheetId="2" r:id="rId2"/>
+    <sheet name="Iteration 1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -730,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39:C39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1469,8 +1469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35:C39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2207,8 +2207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35:C39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
thêm điểm iteration 3
</commit_message>
<xml_diff>
--- a/Diem/Nhom 3.xlsx
+++ b/Diem/Nhom 3.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Version Control" sheetId="1" r:id="rId1"/>
     <sheet name="Project Plan" sheetId="2" r:id="rId2"/>
     <sheet name="Iteration 1" sheetId="3" r:id="rId3"/>
     <sheet name="Iteration 2, Specs and Design" sheetId="4" r:id="rId4"/>
+    <sheet name="Iteration 3" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="130">
   <si>
     <t>Đề tài:</t>
   </si>
@@ -392,6 +393,21 @@
   </si>
   <si>
     <t>giao diện các bạn còn 1 số lỗi do một số nhóm đã góp ý</t>
+  </si>
+  <si>
+    <t>Iteration 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lần insert thứ nhất các bạn làm csdl sai mà không xem xét trước khi nộp </t>
+  </si>
+  <si>
+    <t>các bạn còn làm một số chức năng có sai sót  như mình đã đưa ra, nhưng nhìn chung các bạn có ý thức sửa và làm lại tốt</t>
+  </si>
+  <si>
+    <t>các bạn insert lần 2 add sai dữ liệu</t>
+  </si>
+  <si>
+    <t>các bạn liên tục không nộp bài hoặc không tổng hợp dữ liệu.</t>
   </si>
 </sst>
 </file>
@@ -2986,8 +3002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D54" sqref="A1:F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3758,4 +3774,778 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="2">
+        <f xml:space="preserve"> SUM(D5:D62)</f>
+        <v>420</v>
+      </c>
+      <c r="E3" s="2">
+        <f>SUM(E4:E62)</f>
+        <v>420</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="5"/>
+      <c r="E4">
+        <v>50</v>
+      </c>
+      <c r="F4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="5"/>
+      <c r="E10">
+        <v>40</v>
+      </c>
+      <c r="F10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="5"/>
+      <c r="E16">
+        <v>50</v>
+      </c>
+      <c r="F16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="5"/>
+      <c r="E22">
+        <v>50</v>
+      </c>
+      <c r="F22" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="5"/>
+      <c r="E28">
+        <v>50</v>
+      </c>
+      <c r="F28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" s="4"/>
+      <c r="C34" s="5"/>
+      <c r="E34">
+        <v>50</v>
+      </c>
+      <c r="F34" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D36">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D37">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D38">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D39">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B40" s="4"/>
+      <c r="C40" s="5"/>
+      <c r="E40">
+        <v>30</v>
+      </c>
+      <c r="F40" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D41">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D42">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D43">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D44">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B45" s="4"/>
+      <c r="C45" s="5"/>
+      <c r="E45">
+        <v>50</v>
+      </c>
+      <c r="F45" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D46">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D47">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+      <c r="B48" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D48">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D49">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
+      <c r="B50" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D50">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B51" s="4"/>
+      <c r="C51" s="5"/>
+      <c r="E51">
+        <v>50</v>
+      </c>
+      <c r="F51" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+      <c r="B52" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D52">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+      <c r="B53" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D53">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
+      <c r="B54" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D54">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+      <c r="B55" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D55">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="4"/>
+      <c r="B56" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D56">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B57" s="4"/>
+      <c r="C57" s="5"/>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="4"/>
+      <c r="B58" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C58" t="s">
+        <v>101</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="4"/>
+      <c r="B59" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C59" t="s">
+        <v>103</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="4"/>
+      <c r="B60" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C60" t="s">
+        <v>105</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="4"/>
+      <c r="B61" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C61" t="s">
+        <v>107</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="4"/>
+      <c r="B62" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C62" t="s">
+        <v>109</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update diem nhom 26
</commit_message>
<xml_diff>
--- a/Diem/Nhom 3.xlsx
+++ b/Diem/Nhom 3.xlsx
@@ -4567,8 +4567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4998,7 +4998,7 @@
         <v>112</v>
       </c>
       <c r="D35">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -5010,7 +5010,7 @@
         <v>63</v>
       </c>
       <c r="D36">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -5022,7 +5022,7 @@
         <v>65</v>
       </c>
       <c r="D37">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -5034,7 +5034,7 @@
         <v>67</v>
       </c>
       <c r="D38">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -5046,7 +5046,7 @@
         <v>113</v>
       </c>
       <c r="D39">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>